<commit_message>
wrote lots of code. It was good.
</commit_message>
<xml_diff>
--- a/waveforms.xlsx
+++ b/waveforms.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pulse" sheetId="1" r:id="rId1"/>
     <sheet name="Sine" sheetId="2" r:id="rId2"/>
+    <sheet name="timing" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="e" localSheetId="1">Sine!$A$2</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>x</t>
   </si>
@@ -67,11 +68,20 @@
   <si>
     <t>Adjusted</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,9 +119,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10174,8 +10185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D258"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16666,4 +16677,219 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="A23:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <f>256/(60*A3)</f>
+        <v>4.2666666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B23" si="0">256/(60*A4)</f>
+        <v>2.1333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4222222222222223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0666666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.85333333333333339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.71111111111111114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.60952380952380958</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47407407407407409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.42666666666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38787878787878788</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.35555555555555557</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3282051282051282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30476190476190479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28444444444444444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25098039215686274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.23703703703703705</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22456140350877193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21333333333333335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20317460317460317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>